<commit_message>
Commit with excel upload changes and keylock token issue fixed
</commit_message>
<xml_diff>
--- a/src/assets/templates/QuestionsUpload.xlsx
+++ b/src/assets/templates/QuestionsUpload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B-ANKIT\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyREPO\UAP-UI-GIT\src\assets\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{813EA1C6-AB19-4213-B38C-C9F428F9F406}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8961B9-3FF6-4BDB-93D5-AF4DCBA79C5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{A85804D8-899A-4030-BC99-CA7002D9AF72}"/>
   </bookViews>
@@ -25,30 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>quesCode</t>
-  </si>
-  <si>
-    <t>quesType</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>questionDes</t>
-  </si>
-  <si>
-    <t>createdBy</t>
-  </si>
-  <si>
-    <t>updatedBy</t>
   </si>
   <si>
     <t>duration</t>
   </si>
   <si>
     <t>mark</t>
-  </si>
-  <si>
-    <t>categoryId</t>
   </si>
   <si>
     <t>categoryName</t>
@@ -403,15 +388,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3CA1FD0-F1E9-4BF7-A96E-5EFA7344699A}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -424,21 +418,6 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>